<commit_message>
Added JSON for under_ice_rerun
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
+++ b/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1475,13 +1475,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="291">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
@@ -2167,10 +2167,10 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BR14" sqref="BR14"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2285,24 +2285,24 @@
       <c r="AP1" s="4"/>
       <c r="AQ1" s="4"/>
       <c r="AR1" s="10"/>
-      <c r="AT1" s="57" t="s">
+      <c r="AT1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="57"/>
-      <c r="AY1" s="57" t="s">
+      <c r="AU1" s="59"/>
+      <c r="AV1" s="59"/>
+      <c r="AW1" s="59"/>
+      <c r="AY1" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="57"/>
-      <c r="BB1" s="57"/>
-      <c r="BC1" s="57"/>
-      <c r="BD1" s="57"/>
-      <c r="BF1" s="57" t="s">
+      <c r="AZ1" s="59"/>
+      <c r="BA1" s="59"/>
+      <c r="BB1" s="59"/>
+      <c r="BC1" s="59"/>
+      <c r="BD1" s="59"/>
+      <c r="BF1" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="57"/>
+      <c r="BG1" s="59"/>
       <c r="BI1" s="8" t="s">
         <v>59</v>
       </c>
@@ -2532,10 +2532,10 @@
       <c r="J3" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M3" s="30" t="s">
@@ -2547,10 +2547,10 @@
       <c r="O3" s="40">
         <v>26132363</v>
       </c>
-      <c r="P3" s="58" t="s">
+      <c r="P3" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q3" s="57" t="s">
         <v>124</v>
       </c>
       <c r="R3" t="s">
@@ -2568,7 +2568,7 @@
       <c r="V3" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W3" s="59" t="s">
+      <c r="W3" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X3" s="54" t="s">
@@ -2577,7 +2577,7 @@
       <c r="Y3" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z3" s="59" t="s">
+      <c r="Z3" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA3" s="54" t="s">
@@ -2725,10 +2725,10 @@
       <c r="J4" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="30" t="s">
@@ -2740,10 +2740,10 @@
       <c r="O4" s="40">
         <v>32776170</v>
       </c>
-      <c r="P4" s="58" t="s">
+      <c r="P4" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="Q4" s="58" t="s">
+      <c r="Q4" s="57" t="s">
         <v>126</v>
       </c>
       <c r="R4" t="s">
@@ -2761,7 +2761,7 @@
       <c r="V4" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W4" s="59" t="s">
+      <c r="W4" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X4" s="54" t="s">
@@ -2770,7 +2770,7 @@
       <c r="Y4" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z4" s="59" t="s">
+      <c r="Z4" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA4" s="54" t="s">
@@ -2918,10 +2918,10 @@
       <c r="J5" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M5" s="30" t="s">
@@ -2933,10 +2933,10 @@
       <c r="O5" s="40">
         <v>15374445</v>
       </c>
-      <c r="P5" s="58" t="s">
+      <c r="P5" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="Q5" s="58" t="s">
+      <c r="Q5" s="57" t="s">
         <v>128</v>
       </c>
       <c r="R5" t="s">
@@ -2954,7 +2954,7 @@
       <c r="V5" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W5" s="59" t="s">
+      <c r="W5" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X5" s="54" t="s">
@@ -2963,7 +2963,7 @@
       <c r="Y5" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z5" s="59" t="s">
+      <c r="Z5" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA5" s="54" t="s">
@@ -3111,10 +3111,10 @@
       <c r="J6" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="58" t="s">
+      <c r="L6" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M6" s="30" t="s">
@@ -3126,10 +3126,10 @@
       <c r="O6" s="40">
         <v>20236324</v>
       </c>
-      <c r="P6" s="58" t="s">
+      <c r="P6" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="Q6" s="58" t="s">
+      <c r="Q6" s="57" t="s">
         <v>130</v>
       </c>
       <c r="R6" t="s">
@@ -3147,7 +3147,7 @@
       <c r="V6" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W6" s="59" t="s">
+      <c r="W6" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X6" s="54" t="s">
@@ -3156,7 +3156,7 @@
       <c r="Y6" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z6" s="59" t="s">
+      <c r="Z6" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA6" s="54" t="s">
@@ -3304,10 +3304,10 @@
       <c r="J7" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="K7" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="58" t="s">
+      <c r="L7" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M7" s="30" t="s">
@@ -3319,10 +3319,10 @@
       <c r="O7" s="40">
         <v>23475092</v>
       </c>
-      <c r="P7" s="58" t="s">
+      <c r="P7" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="Q7" s="58" t="s">
+      <c r="Q7" s="57" t="s">
         <v>132</v>
       </c>
       <c r="R7" t="s">
@@ -3340,7 +3340,7 @@
       <c r="V7" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W7" s="59" t="s">
+      <c r="W7" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X7" s="54" t="s">
@@ -3349,7 +3349,7 @@
       <c r="Y7" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z7" s="59" t="s">
+      <c r="Z7" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA7" s="54" t="s">
@@ -3497,10 +3497,10 @@
       <c r="J8" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L8" s="58" t="s">
+      <c r="L8" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M8" s="30" t="s">
@@ -3512,10 +3512,10 @@
       <c r="O8" s="40">
         <v>19019111</v>
       </c>
-      <c r="P8" s="58" t="s">
+      <c r="P8" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="Q8" s="58" t="s">
+      <c r="Q8" s="57" t="s">
         <v>134</v>
       </c>
       <c r="R8" t="s">
@@ -3533,7 +3533,7 @@
       <c r="V8" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W8" s="59" t="s">
+      <c r="W8" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X8" s="54" t="s">
@@ -3542,7 +3542,7 @@
       <c r="Y8" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z8" s="59" t="s">
+      <c r="Z8" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA8" s="54" t="s">
@@ -3690,10 +3690,10 @@
       <c r="J9" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M9" s="30" t="s">
@@ -3705,10 +3705,10 @@
       <c r="O9" s="40">
         <v>23417974</v>
       </c>
-      <c r="P9" s="58" t="s">
+      <c r="P9" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="Q9" s="58" t="s">
+      <c r="Q9" s="57" t="s">
         <v>136</v>
       </c>
       <c r="R9" t="s">
@@ -3726,7 +3726,7 @@
       <c r="V9" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W9" s="59" t="s">
+      <c r="W9" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X9" s="54" t="s">
@@ -3735,7 +3735,7 @@
       <c r="Y9" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z9" s="59" t="s">
+      <c r="Z9" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA9" s="54" t="s">
@@ -3883,10 +3883,10 @@
       <c r="J10" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M10" s="30" t="s">
@@ -3898,10 +3898,10 @@
       <c r="O10" s="40">
         <v>21959015</v>
       </c>
-      <c r="P10" s="58" t="s">
+      <c r="P10" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="Q10" s="58" t="s">
+      <c r="Q10" s="57" t="s">
         <v>138</v>
       </c>
       <c r="R10" t="s">
@@ -3919,7 +3919,7 @@
       <c r="V10" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W10" s="59" t="s">
+      <c r="W10" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X10" s="54" t="s">
@@ -3928,7 +3928,7 @@
       <c r="Y10" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z10" s="59" t="s">
+      <c r="Z10" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA10" s="54" t="s">
@@ -4053,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="23">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>64</v>
@@ -4076,10 +4076,10 @@
       <c r="J11" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M11" s="30" t="s">
@@ -4091,10 +4091,10 @@
       <c r="O11" s="40">
         <v>19349699</v>
       </c>
-      <c r="P11" s="58" t="s">
+      <c r="P11" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="Q11" s="58" t="s">
+      <c r="Q11" s="57" t="s">
         <v>140</v>
       </c>
       <c r="R11" t="s">
@@ -4112,7 +4112,7 @@
       <c r="V11" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W11" s="59" t="s">
+      <c r="W11" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X11" s="54" t="s">
@@ -4121,7 +4121,7 @@
       <c r="Y11" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z11" s="59" t="s">
+      <c r="Z11" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA11" s="54" t="s">
@@ -4246,7 +4246,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>64</v>
@@ -4269,10 +4269,10 @@
       <c r="J12" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M12" s="30" t="s">
@@ -4284,10 +4284,10 @@
       <c r="O12" s="40">
         <v>24640452</v>
       </c>
-      <c r="P12" s="58" t="s">
+      <c r="P12" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="Q12" s="58" t="s">
+      <c r="Q12" s="57" t="s">
         <v>142</v>
       </c>
       <c r="R12" t="s">
@@ -4305,7 +4305,7 @@
       <c r="V12" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W12" s="59" t="s">
+      <c r="W12" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X12" s="54" t="s">
@@ -4314,7 +4314,7 @@
       <c r="Y12" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z12" s="59" t="s">
+      <c r="Z12" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA12" s="54" t="s">
@@ -4439,7 +4439,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="23">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>64</v>
@@ -4462,10 +4462,10 @@
       <c r="J13" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L13" s="58" t="s">
+      <c r="L13" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M13" s="30" t="s">
@@ -4477,10 +4477,10 @@
       <c r="O13" s="40">
         <v>22292795</v>
       </c>
-      <c r="P13" s="58" t="s">
+      <c r="P13" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" s="58" t="s">
+      <c r="Q13" s="57" t="s">
         <v>144</v>
       </c>
       <c r="R13" t="s">
@@ -4498,7 +4498,7 @@
       <c r="V13" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W13" s="59" t="s">
+      <c r="W13" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X13" s="54" t="s">
@@ -4507,7 +4507,7 @@
       <c r="Y13" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z13" s="59" t="s">
+      <c r="Z13" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA13" s="54" t="s">
@@ -4632,7 +4632,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>64</v>
@@ -4655,10 +4655,10 @@
       <c r="J14" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L14" s="58" t="s">
+      <c r="L14" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M14" s="30" t="s">
@@ -4670,10 +4670,10 @@
       <c r="O14" s="40">
         <v>24336672</v>
       </c>
-      <c r="P14" s="58" t="s">
+      <c r="P14" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="Q14" s="58" t="s">
+      <c r="Q14" s="57" t="s">
         <v>146</v>
       </c>
       <c r="R14" t="s">
@@ -4691,7 +4691,7 @@
       <c r="V14" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W14" s="59" t="s">
+      <c r="W14" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X14" s="54" t="s">
@@ -4700,7 +4700,7 @@
       <c r="Y14" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z14" s="59" t="s">
+      <c r="Z14" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA14" s="54" t="s">
@@ -4825,7 +4825,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="23">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>64</v>
@@ -4848,10 +4848,10 @@
       <c r="J15" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L15" s="58" t="s">
+      <c r="L15" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M15" s="30" t="s">
@@ -4863,10 +4863,10 @@
       <c r="O15" s="40">
         <v>22153770</v>
       </c>
-      <c r="P15" s="58" t="s">
+      <c r="P15" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="Q15" s="58" t="s">
+      <c r="Q15" s="57" t="s">
         <v>148</v>
       </c>
       <c r="R15" t="s">
@@ -4884,7 +4884,7 @@
       <c r="V15" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W15" s="59" t="s">
+      <c r="W15" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X15" s="54" t="s">
@@ -4893,7 +4893,7 @@
       <c r="Y15" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z15" s="59" t="s">
+      <c r="Z15" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA15" s="54" t="s">
@@ -5018,7 +5018,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="23">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>64</v>
@@ -5041,10 +5041,10 @@
       <c r="J16" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L16" s="58" t="s">
+      <c r="L16" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M16" s="30" t="s">
@@ -5056,10 +5056,10 @@
       <c r="O16" s="40">
         <v>23514431</v>
       </c>
-      <c r="P16" s="58" t="s">
+      <c r="P16" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="Q16" s="58" t="s">
+      <c r="Q16" s="57" t="s">
         <v>150</v>
       </c>
       <c r="R16" t="s">
@@ -5077,7 +5077,7 @@
       <c r="V16" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W16" s="59" t="s">
+      <c r="W16" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X16" s="54" t="s">
@@ -5086,7 +5086,7 @@
       <c r="Y16" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z16" s="59" t="s">
+      <c r="Z16" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA16" s="54" t="s">
@@ -5211,7 +5211,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="23">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>64</v>
@@ -5234,10 +5234,10 @@
       <c r="J17" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="K17" s="58" t="s">
+      <c r="K17" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="58" t="s">
+      <c r="L17" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M17" s="30" t="s">
@@ -5249,10 +5249,10 @@
       <c r="O17" s="40">
         <v>25239007</v>
       </c>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="Q17" s="58" t="s">
+      <c r="Q17" s="57" t="s">
         <v>152</v>
       </c>
       <c r="R17" t="s">
@@ -5270,7 +5270,7 @@
       <c r="V17" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W17" s="59" t="s">
+      <c r="W17" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X17" s="54" t="s">
@@ -5279,7 +5279,7 @@
       <c r="Y17" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z17" s="59" t="s">
+      <c r="Z17" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA17" s="54" t="s">
@@ -5404,7 +5404,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="23">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>64</v>
@@ -5427,10 +5427,10 @@
       <c r="J18" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="58" t="s">
+      <c r="K18" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L18" s="58" t="s">
+      <c r="L18" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M18" s="30" t="s">
@@ -5442,10 +5442,10 @@
       <c r="O18" s="40">
         <v>26888537</v>
       </c>
-      <c r="P18" s="58" t="s">
+      <c r="P18" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="Q18" s="58" t="s">
+      <c r="Q18" s="57" t="s">
         <v>154</v>
       </c>
       <c r="R18" t="s">
@@ -5463,7 +5463,7 @@
       <c r="V18" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W18" s="59" t="s">
+      <c r="W18" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X18" s="54" t="s">
@@ -5472,7 +5472,7 @@
       <c r="Y18" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z18" s="59" t="s">
+      <c r="Z18" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA18" s="54" t="s">
@@ -5597,7 +5597,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="23">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>64</v>
@@ -5620,10 +5620,10 @@
       <c r="J19" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="K19" s="58" t="s">
+      <c r="K19" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L19" s="58" t="s">
+      <c r="L19" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M19" s="30" t="s">
@@ -5635,10 +5635,10 @@
       <c r="O19" s="40">
         <v>24099741</v>
       </c>
-      <c r="P19" s="58" t="s">
+      <c r="P19" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="Q19" s="58" t="s">
+      <c r="Q19" s="57" t="s">
         <v>156</v>
       </c>
       <c r="R19" t="s">
@@ -5656,7 +5656,7 @@
       <c r="V19" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W19" s="59" t="s">
+      <c r="W19" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X19" s="54" t="s">
@@ -5665,7 +5665,7 @@
       <c r="Y19" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z19" s="59" t="s">
+      <c r="Z19" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA19" s="54" t="s">
@@ -5788,7 +5788,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="23">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>64</v>
@@ -5811,10 +5811,10 @@
       <c r="J20" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="K20" s="58" t="s">
+      <c r="K20" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L20" s="58" t="s">
+      <c r="L20" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M20" s="30" t="s">
@@ -5826,10 +5826,10 @@
       <c r="O20" s="40">
         <v>25131709</v>
       </c>
-      <c r="P20" s="58" t="s">
+      <c r="P20" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="Q20" s="58" t="s">
+      <c r="Q20" s="57" t="s">
         <v>158</v>
       </c>
       <c r="R20" t="s">
@@ -5847,7 +5847,7 @@
       <c r="V20" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W20" s="59" t="s">
+      <c r="W20" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X20" s="54" t="s">
@@ -5856,7 +5856,7 @@
       <c r="Y20" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z20" s="59" t="s">
+      <c r="Z20" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA20" s="54" t="s">
@@ -5979,7 +5979,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="23">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>64</v>
@@ -6002,10 +6002,10 @@
       <c r="J21" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="K21" s="58" t="s">
+      <c r="K21" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="58" t="s">
+      <c r="L21" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M21" s="30" t="s">
@@ -6017,10 +6017,10 @@
       <c r="O21" s="40">
         <v>25333059</v>
       </c>
-      <c r="P21" s="58" t="s">
+      <c r="P21" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="Q21" s="58" t="s">
+      <c r="Q21" s="57" t="s">
         <v>160</v>
       </c>
       <c r="R21" t="s">
@@ -6038,7 +6038,7 @@
       <c r="V21" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W21" s="59" t="s">
+      <c r="W21" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X21" s="54" t="s">
@@ -6047,7 +6047,7 @@
       <c r="Y21" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z21" s="59" t="s">
+      <c r="Z21" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA21" s="54" t="s">
@@ -6170,7 +6170,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="23">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>64</v>
@@ -6193,10 +6193,10 @@
       <c r="J22" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="K22" s="58" t="s">
+      <c r="K22" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L22" s="58" t="s">
+      <c r="L22" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M22" s="30" t="s">
@@ -6208,10 +6208,10 @@
       <c r="O22" s="40">
         <v>23643065</v>
       </c>
-      <c r="P22" s="58" t="s">
+      <c r="P22" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="Q22" s="58" t="s">
+      <c r="Q22" s="57" t="s">
         <v>162</v>
       </c>
       <c r="R22" t="s">
@@ -6229,7 +6229,7 @@
       <c r="V22" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W22" s="59" t="s">
+      <c r="W22" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X22" s="54" t="s">
@@ -6238,7 +6238,7 @@
       <c r="Y22" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z22" s="59" t="s">
+      <c r="Z22" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA22" s="54" t="s">
@@ -6361,7 +6361,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="23">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>64</v>
@@ -6384,10 +6384,10 @@
       <c r="J23" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L23" s="58" t="s">
+      <c r="L23" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M23" s="30" t="s">
@@ -6399,10 +6399,10 @@
       <c r="O23" s="40">
         <v>23126069</v>
       </c>
-      <c r="P23" s="58" t="s">
+      <c r="P23" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="Q23" s="58" t="s">
+      <c r="Q23" s="57" t="s">
         <v>164</v>
       </c>
       <c r="R23" t="s">
@@ -6420,7 +6420,7 @@
       <c r="V23" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W23" s="59" t="s">
+      <c r="W23" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X23" s="54" t="s">
@@ -6429,7 +6429,7 @@
       <c r="Y23" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z23" s="59" t="s">
+      <c r="Z23" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA23" s="54" t="s">
@@ -6552,7 +6552,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="23">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>64</v>
@@ -6575,10 +6575,10 @@
       <c r="J24" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="K24" s="58" t="s">
+      <c r="K24" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L24" s="58" t="s">
+      <c r="L24" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M24" s="30" t="s">
@@ -6590,10 +6590,10 @@
       <c r="O24" s="40">
         <v>21665592</v>
       </c>
-      <c r="P24" s="58" t="s">
+      <c r="P24" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="Q24" s="58" t="s">
+      <c r="Q24" s="57" t="s">
         <v>166</v>
       </c>
       <c r="R24" t="s">
@@ -6611,7 +6611,7 @@
       <c r="V24" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W24" s="59" t="s">
+      <c r="W24" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X24" s="54" t="s">
@@ -6620,7 +6620,7 @@
       <c r="Y24" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z24" s="59" t="s">
+      <c r="Z24" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA24" s="54" t="s">
@@ -6743,7 +6743,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="23">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>64</v>
@@ -6766,10 +6766,10 @@
       <c r="J25" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="K25" s="58" t="s">
+      <c r="K25" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="L25" s="58" t="s">
+      <c r="L25" s="57" t="s">
         <v>122</v>
       </c>
       <c r="M25" s="30" t="s">
@@ -6781,10 +6781,10 @@
       <c r="O25" s="40">
         <v>24804911</v>
       </c>
-      <c r="P25" s="58" t="s">
+      <c r="P25" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="Q25" s="58" t="s">
+      <c r="Q25" s="57" t="s">
         <v>168</v>
       </c>
       <c r="R25" t="s">
@@ -6802,7 +6802,7 @@
       <c r="V25" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="W25" s="59" t="s">
+      <c r="W25" s="58" t="s">
         <v>193</v>
       </c>
       <c r="X25" s="54" t="s">
@@ -6811,7 +6811,7 @@
       <c r="Y25" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="Z25" s="59" t="s">
+      <c r="Z25" s="58" t="s">
         <v>195</v>
       </c>
       <c r="AA25" s="54" t="s">
@@ -6930,19 +6930,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -6960,14 +6950,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Added sra ids for under_ice_rerun
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
+++ b/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51100" windowHeight="13820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51100" windowHeight="18760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="242">
   <si>
     <t>Country</t>
   </si>
@@ -843,7 +843,16 @@
     <t>Lake near Krokom</t>
   </si>
   <si>
-    <t>PRJNAXXXXXX</t>
+    <t>PRJNA417044</t>
+  </si>
+  <si>
+    <t>SAMN07975454</t>
+  </si>
+  <si>
+    <t>SAMN07975455</t>
+  </si>
+  <si>
+    <t>SAMN07975456</t>
   </si>
 </sst>
 </file>
@@ -2167,10 +2176,10 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="BG29" sqref="BG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2665,11 +2674,11 @@
       <c r="BE3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF3" s="25" t="s">
+      <c r="BF3" t="s">
         <v>238</v>
       </c>
-      <c r="BG3" s="25" t="s">
-        <v>238</v>
+      <c r="BG3" t="s">
+        <v>239</v>
       </c>
       <c r="BI3">
         <v>0.5</v>
@@ -2858,11 +2867,11 @@
       <c r="BE4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF4" s="25" t="s">
+      <c r="BF4" t="s">
         <v>238</v>
       </c>
-      <c r="BG4" s="25" t="s">
-        <v>238</v>
+      <c r="BG4" t="s">
+        <v>239</v>
       </c>
       <c r="BI4">
         <v>0.9</v>
@@ -3051,11 +3060,11 @@
       <c r="BE5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF5" s="25" t="s">
+      <c r="BF5" t="s">
         <v>238</v>
       </c>
-      <c r="BG5" s="25" t="s">
-        <v>238</v>
+      <c r="BG5" t="s">
+        <v>239</v>
       </c>
       <c r="BI5">
         <v>1.1000000000000001</v>
@@ -3244,11 +3253,11 @@
       <c r="BE6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF6" s="25" t="s">
+      <c r="BF6" t="s">
         <v>238</v>
       </c>
-      <c r="BG6" s="25" t="s">
-        <v>238</v>
+      <c r="BG6" t="s">
+        <v>239</v>
       </c>
       <c r="BI6">
         <v>1.3</v>
@@ -3437,11 +3446,11 @@
       <c r="BE7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF7" s="25" t="s">
+      <c r="BF7" t="s">
         <v>238</v>
       </c>
-      <c r="BG7" s="25" t="s">
-        <v>238</v>
+      <c r="BG7" t="s">
+        <v>239</v>
       </c>
       <c r="BI7">
         <v>1.5</v>
@@ -3630,11 +3639,11 @@
       <c r="BE8" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF8" s="25" t="s">
+      <c r="BF8" t="s">
         <v>238</v>
       </c>
-      <c r="BG8" s="25" t="s">
-        <v>238</v>
+      <c r="BG8" t="s">
+        <v>239</v>
       </c>
       <c r="BI8">
         <v>2</v>
@@ -3823,11 +3832,11 @@
       <c r="BE9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF9" s="25" t="s">
+      <c r="BF9" t="s">
         <v>238</v>
       </c>
-      <c r="BG9" s="25" t="s">
-        <v>238</v>
+      <c r="BG9" t="s">
+        <v>239</v>
       </c>
       <c r="BI9">
         <v>2.5</v>
@@ -4016,11 +4025,11 @@
       <c r="BE10" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF10" s="25" t="s">
+      <c r="BF10" t="s">
         <v>238</v>
       </c>
-      <c r="BG10" s="25" t="s">
-        <v>238</v>
+      <c r="BG10" t="s">
+        <v>239</v>
       </c>
       <c r="BI10">
         <v>3.5</v>
@@ -4209,11 +4218,11 @@
       <c r="BE11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF11" s="25" t="s">
+      <c r="BF11" t="s">
         <v>238</v>
       </c>
-      <c r="BG11" s="25" t="s">
-        <v>238</v>
+      <c r="BG11" t="s">
+        <v>240</v>
       </c>
       <c r="BI11">
         <v>0.6</v>
@@ -4402,11 +4411,11 @@
       <c r="BE12" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF12" s="25" t="s">
+      <c r="BF12" t="s">
         <v>238</v>
       </c>
-      <c r="BG12" s="25" t="s">
-        <v>238</v>
+      <c r="BG12" t="s">
+        <v>240</v>
       </c>
       <c r="BI12">
         <v>0.8</v>
@@ -4595,11 +4604,11 @@
       <c r="BE13" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF13" s="25" t="s">
+      <c r="BF13" t="s">
         <v>238</v>
       </c>
-      <c r="BG13" s="25" t="s">
-        <v>238</v>
+      <c r="BG13" t="s">
+        <v>240</v>
       </c>
       <c r="BI13">
         <v>1</v>
@@ -4788,11 +4797,11 @@
       <c r="BE14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF14" s="25" t="s">
+      <c r="BF14" t="s">
         <v>238</v>
       </c>
-      <c r="BG14" s="25" t="s">
-        <v>238</v>
+      <c r="BG14" t="s">
+        <v>240</v>
       </c>
       <c r="BI14">
         <v>1.2</v>
@@ -4981,11 +4990,11 @@
       <c r="BE15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF15" s="25" t="s">
+      <c r="BF15" t="s">
         <v>238</v>
       </c>
-      <c r="BG15" s="25" t="s">
-        <v>238</v>
+      <c r="BG15" t="s">
+        <v>240</v>
       </c>
       <c r="BI15">
         <v>1.5</v>
@@ -5174,11 +5183,11 @@
       <c r="BE16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF16" s="25" t="s">
+      <c r="BF16" t="s">
         <v>238</v>
       </c>
-      <c r="BG16" s="25" t="s">
-        <v>238</v>
+      <c r="BG16" t="s">
+        <v>240</v>
       </c>
       <c r="BI16">
         <v>1.8</v>
@@ -5367,11 +5376,11 @@
       <c r="BE17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF17" s="25" t="s">
+      <c r="BF17" t="s">
         <v>238</v>
       </c>
-      <c r="BG17" s="25" t="s">
-        <v>238</v>
+      <c r="BG17" t="s">
+        <v>240</v>
       </c>
       <c r="BI17">
         <v>2.2999999999999998</v>
@@ -5560,11 +5569,11 @@
       <c r="BE18" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF18" s="25" t="s">
+      <c r="BF18" t="s">
         <v>238</v>
       </c>
-      <c r="BG18" s="25" t="s">
-        <v>238</v>
+      <c r="BG18" t="s">
+        <v>240</v>
       </c>
       <c r="BI18">
         <v>2.6</v>
@@ -5753,11 +5762,11 @@
       <c r="BE19" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF19" s="25" t="s">
+      <c r="BF19" t="s">
         <v>238</v>
       </c>
-      <c r="BG19" s="25" t="s">
-        <v>238</v>
+      <c r="BG19" t="s">
+        <v>241</v>
       </c>
       <c r="BI19">
         <v>0.45</v>
@@ -5944,11 +5953,11 @@
       <c r="BE20" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF20" s="25" t="s">
+      <c r="BF20" t="s">
         <v>238</v>
       </c>
-      <c r="BG20" s="25" t="s">
-        <v>238</v>
+      <c r="BG20" t="s">
+        <v>241</v>
       </c>
       <c r="BI20">
         <v>0.75</v>
@@ -6135,11 +6144,11 @@
       <c r="BE21" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF21" s="25" t="s">
+      <c r="BF21" t="s">
         <v>238</v>
       </c>
-      <c r="BG21" s="25" t="s">
-        <v>238</v>
+      <c r="BG21" t="s">
+        <v>241</v>
       </c>
       <c r="BI21">
         <v>1.05</v>
@@ -6326,11 +6335,11 @@
       <c r="BE22" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF22" s="25" t="s">
+      <c r="BF22" t="s">
         <v>238</v>
       </c>
-      <c r="BG22" s="25" t="s">
-        <v>238</v>
+      <c r="BG22" t="s">
+        <v>241</v>
       </c>
       <c r="BI22">
         <v>1.35</v>
@@ -6517,11 +6526,11 @@
       <c r="BE23" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF23" s="25" t="s">
+      <c r="BF23" t="s">
         <v>238</v>
       </c>
-      <c r="BG23" s="25" t="s">
-        <v>238</v>
+      <c r="BG23" t="s">
+        <v>241</v>
       </c>
       <c r="BI23">
         <v>1.95</v>
@@ -6708,11 +6717,11 @@
       <c r="BE24" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF24" s="25" t="s">
+      <c r="BF24" t="s">
         <v>238</v>
       </c>
-      <c r="BG24" s="25" t="s">
-        <v>238</v>
+      <c r="BG24" t="s">
+        <v>241</v>
       </c>
       <c r="BI24">
         <v>2.95</v>
@@ -6899,11 +6908,11 @@
       <c r="BE25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="BF25" s="25" t="s">
+      <c r="BF25" t="s">
         <v>238</v>
       </c>
-      <c r="BG25" s="25" t="s">
-        <v>238</v>
+      <c r="BG25" t="s">
+        <v>241</v>
       </c>
       <c r="BI25">
         <v>3.25</v>
@@ -6930,9 +6939,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -6950,24 +6969,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Added sra ids for under_ice_rerun bis
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
+++ b/metadata/excel/projects/uppsala_universitet/under_ice_rerun/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -327,9 +327,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Illumina HiSeq</t>
-  </si>
-  <si>
     <t>RANDOM</t>
   </si>
   <si>
@@ -834,9 +831,6 @@
     <t>Lake near Skalstugan</t>
   </si>
   <si>
-    <t>Water was sampled from under the lake's ice cover using Limnos sampler. Water was prefiltered using a 50 µm sieve and freeze dried. DNA was extracted from dried material using PowerSoil DNA extraction kit.</t>
-  </si>
-  <si>
     <t>Lake near Ånn</t>
   </si>
   <si>
@@ -853,6 +847,12 @@
   </si>
   <si>
     <t>SAMN07975456</t>
+  </si>
+  <si>
+    <t>Water was sampled from under the lake's ice cover using Limnos sampler. Water was prefiltered using a 50 um sieve and freeze dried. DNA was extracted from dried material using PowerSoil DNA extraction kit.</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 1000</t>
   </si>
 </sst>
 </file>
@@ -2176,10 +2176,10 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BG29" sqref="BG29"/>
+      <selection pane="bottomLeft" activeCell="AQ16" sqref="AQ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2223,7 +2223,7 @@
     <col min="38" max="38" width="10.83203125" customWidth="1"/>
     <col min="39" max="39" width="14" customWidth="1"/>
     <col min="40" max="40" width="13.1640625" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" customWidth="1"/>
+    <col min="41" max="41" width="18.83203125" customWidth="1"/>
     <col min="42" max="42" width="11.6640625" customWidth="1"/>
     <col min="43" max="43" width="12.1640625" customWidth="1"/>
     <col min="44" max="44" width="13" customWidth="1"/>
@@ -2524,28 +2524,28 @@
         <v>64</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="I3" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="J3" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="30" t="s">
-        <v>98</v>
-      </c>
       <c r="K3" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L3" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M3" s="30" t="s">
         <v>40</v>
@@ -2557,55 +2557,55 @@
         <v>26132363</v>
       </c>
       <c r="P3" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q3" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="Q3" s="57" t="s">
-        <v>124</v>
-      </c>
       <c r="R3" t="s">
         <v>40</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V3" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W3" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X3" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y3" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z3" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W3" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X3" s="54" t="s">
+      <c r="AA3" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="Y3" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z3" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA3" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" s="56" t="s">
-        <v>198</v>
-      </c>
       <c r="AD3" s="53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE3" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF3" s="53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AG3" s="53">
         <v>28.768324649687713</v>
@@ -2615,13 +2615,13 @@
         <v>40</v>
       </c>
       <c r="AJ3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK3" t="s">
         <v>3</v>
       </c>
       <c r="AL3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM3" t="s">
         <v>58</v>
@@ -2630,10 +2630,10 @@
         <v>4</v>
       </c>
       <c r="AO3" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ3">
         <v>124</v>
@@ -2642,16 +2642,16 @@
         <v>124</v>
       </c>
       <c r="AT3" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU3" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU3" s="55" t="s">
+      <c r="AV3" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV3" s="55" t="s">
+      <c r="AW3" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW3" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY3" s="24">
         <v>40254</v>
@@ -2663,22 +2663,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB3" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC3" t="s">
         <v>233</v>
       </c>
-      <c r="BC3" t="s">
-        <v>234</v>
-      </c>
       <c r="BD3" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE3" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI3">
         <v>0.5</v>
@@ -2717,28 +2717,28 @@
         <v>64</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="I4" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J4" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L4" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M4" s="30" t="s">
         <v>40</v>
@@ -2750,55 +2750,55 @@
         <v>32776170</v>
       </c>
       <c r="P4" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q4" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="Q4" s="57" t="s">
-        <v>126</v>
-      </c>
       <c r="R4" t="s">
         <v>40</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T4" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V4" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W4" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X4" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y4" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z4" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W4" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X4" s="54" t="s">
+      <c r="AA4" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="Y4" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z4" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA4" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="56" t="s">
-        <v>198</v>
-      </c>
       <c r="AD4" s="53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE4" s="56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF4" s="53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AG4" s="53">
         <v>11.041282374896175</v>
@@ -2808,13 +2808,13 @@
         <v>40</v>
       </c>
       <c r="AJ4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK4" t="s">
         <v>3</v>
       </c>
       <c r="AL4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM4" t="s">
         <v>58</v>
@@ -2823,10 +2823,10 @@
         <v>4</v>
       </c>
       <c r="AO4" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ4">
         <v>124</v>
@@ -2835,16 +2835,16 @@
         <v>124</v>
       </c>
       <c r="AT4" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU4" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU4" s="55" t="s">
+      <c r="AV4" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV4" s="55" t="s">
+      <c r="AW4" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW4" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY4" s="24">
         <v>40254</v>
@@ -2856,22 +2856,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB4" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC4" t="s">
         <v>233</v>
       </c>
-      <c r="BC4" t="s">
-        <v>234</v>
-      </c>
       <c r="BD4" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI4">
         <v>0.9</v>
@@ -2910,28 +2910,28 @@
         <v>64</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="I5" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J5" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K5" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L5" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M5" s="30" t="s">
         <v>40</v>
@@ -2943,55 +2943,55 @@
         <v>15374445</v>
       </c>
       <c r="P5" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q5" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="Q5" s="57" t="s">
-        <v>128</v>
-      </c>
       <c r="R5" t="s">
         <v>40</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V5" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W5" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X5" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y5" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z5" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W5" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X5" s="54" t="s">
+      <c r="AA5" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="Y5" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z5" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA5" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="56" t="s">
-        <v>198</v>
-      </c>
       <c r="AD5" s="53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE5" s="56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF5" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG5" s="53">
         <v>30.481861428432737</v>
@@ -3001,13 +3001,13 @@
         <v>40</v>
       </c>
       <c r="AJ5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK5" t="s">
         <v>3</v>
       </c>
       <c r="AL5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM5" t="s">
         <v>58</v>
@@ -3016,10 +3016,10 @@
         <v>4</v>
       </c>
       <c r="AO5" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ5">
         <v>124</v>
@@ -3028,16 +3028,16 @@
         <v>124</v>
       </c>
       <c r="AT5" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU5" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU5" s="55" t="s">
+      <c r="AV5" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV5" s="55" t="s">
+      <c r="AW5" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW5" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY5" s="24">
         <v>40254</v>
@@ -3049,22 +3049,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB5" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC5" t="s">
         <v>233</v>
       </c>
-      <c r="BC5" t="s">
-        <v>234</v>
-      </c>
       <c r="BD5" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE5" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI5">
         <v>1.1000000000000001</v>
@@ -3103,28 +3103,28 @@
         <v>64</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="I6" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J6" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K6" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L6" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M6" s="30" t="s">
         <v>40</v>
@@ -3136,55 +3136,55 @@
         <v>20236324</v>
       </c>
       <c r="P6" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="Q6" s="57" t="s">
-        <v>130</v>
-      </c>
       <c r="R6" t="s">
         <v>40</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V6" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W6" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X6" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y6" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z6" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W6" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X6" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y6" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z6" s="58" t="s">
+      <c r="AA6" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA6" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC6" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD6" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE6" s="56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF6" s="53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AG6" s="53">
         <v>9.7737937283583065</v>
@@ -3194,13 +3194,13 @@
         <v>40</v>
       </c>
       <c r="AJ6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK6" t="s">
         <v>3</v>
       </c>
       <c r="AL6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM6" t="s">
         <v>58</v>
@@ -3209,10 +3209,10 @@
         <v>4</v>
       </c>
       <c r="AO6" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ6">
         <v>124</v>
@@ -3221,16 +3221,16 @@
         <v>124</v>
       </c>
       <c r="AT6" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU6" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU6" s="55" t="s">
+      <c r="AV6" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV6" s="55" t="s">
+      <c r="AW6" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW6" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY6" s="24">
         <v>40254</v>
@@ -3242,22 +3242,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB6" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC6" t="s">
         <v>233</v>
       </c>
-      <c r="BC6" t="s">
-        <v>234</v>
-      </c>
       <c r="BD6" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE6" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI6">
         <v>1.3</v>
@@ -3296,28 +3296,28 @@
         <v>64</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="I7" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J7" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K7" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L7" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M7" s="30" t="s">
         <v>40</v>
@@ -3329,55 +3329,55 @@
         <v>23475092</v>
       </c>
       <c r="P7" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q7" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="Q7" s="57" t="s">
-        <v>132</v>
-      </c>
       <c r="R7" t="s">
         <v>40</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V7" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W7" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X7" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y7" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z7" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W7" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X7" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y7" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z7" s="58" t="s">
+      <c r="AA7" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA7" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC7" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD7" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE7" s="56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AF7" s="53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AG7" s="53">
         <v>11.207943647994133</v>
@@ -3387,13 +3387,13 @@
         <v>40</v>
       </c>
       <c r="AJ7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK7" t="s">
         <v>3</v>
       </c>
       <c r="AL7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM7" t="s">
         <v>58</v>
@@ -3402,10 +3402,10 @@
         <v>4</v>
       </c>
       <c r="AO7" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ7">
         <v>124</v>
@@ -3414,16 +3414,16 @@
         <v>124</v>
       </c>
       <c r="AT7" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU7" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU7" s="55" t="s">
+      <c r="AV7" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV7" s="55" t="s">
+      <c r="AW7" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW7" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY7" s="24">
         <v>40254</v>
@@ -3435,22 +3435,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB7" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC7" t="s">
         <v>233</v>
       </c>
-      <c r="BC7" t="s">
-        <v>234</v>
-      </c>
       <c r="BD7" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE7" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI7">
         <v>1.5</v>
@@ -3489,28 +3489,28 @@
         <v>64</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="I8" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I8" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J8" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K8" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L8" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M8" s="30" t="s">
         <v>40</v>
@@ -3522,55 +3522,55 @@
         <v>19019111</v>
       </c>
       <c r="P8" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="Q8" s="57" t="s">
-        <v>134</v>
-      </c>
       <c r="R8" t="s">
         <v>40</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V8" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W8" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X8" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y8" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z8" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W8" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X8" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y8" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z8" s="58" t="s">
+      <c r="AA8" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA8" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC8" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD8" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE8" s="56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AF8" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG8" s="53">
         <v>11.713860392867545</v>
@@ -3580,13 +3580,13 @@
         <v>40</v>
       </c>
       <c r="AJ8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK8" t="s">
         <v>3</v>
       </c>
       <c r="AL8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM8" t="s">
         <v>58</v>
@@ -3595,10 +3595,10 @@
         <v>4</v>
       </c>
       <c r="AO8" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ8">
         <v>124</v>
@@ -3607,16 +3607,16 @@
         <v>124</v>
       </c>
       <c r="AT8" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU8" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU8" s="55" t="s">
+      <c r="AV8" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV8" s="55" t="s">
+      <c r="AW8" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW8" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY8" s="24">
         <v>40254</v>
@@ -3628,22 +3628,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB8" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC8" t="s">
         <v>233</v>
       </c>
-      <c r="BC8" t="s">
-        <v>234</v>
-      </c>
       <c r="BD8" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE8" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI8">
         <v>2</v>
@@ -3682,28 +3682,28 @@
         <v>64</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="I9" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J9" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L9" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M9" s="30" t="s">
         <v>40</v>
@@ -3715,55 +3715,55 @@
         <v>23417974</v>
       </c>
       <c r="P9" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q9" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="Q9" s="57" t="s">
-        <v>136</v>
-      </c>
       <c r="R9" t="s">
         <v>40</v>
       </c>
       <c r="S9" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V9" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W9" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X9" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y9" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z9" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W9" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X9" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y9" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z9" s="58" t="s">
+      <c r="AA9" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA9" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC9" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD9" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE9" s="56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AF9" s="53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG9" s="53">
         <v>6.0511526056330434</v>
@@ -3773,13 +3773,13 @@
         <v>40</v>
       </c>
       <c r="AJ9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK9" t="s">
         <v>3</v>
       </c>
       <c r="AL9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM9" t="s">
         <v>58</v>
@@ -3788,10 +3788,10 @@
         <v>4</v>
       </c>
       <c r="AO9" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ9">
         <v>124</v>
@@ -3800,16 +3800,16 @@
         <v>124</v>
       </c>
       <c r="AT9" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU9" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU9" s="55" t="s">
+      <c r="AV9" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV9" s="55" t="s">
+      <c r="AW9" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW9" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY9" s="24">
         <v>40254</v>
@@ -3821,22 +3821,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB9" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC9" t="s">
         <v>233</v>
       </c>
-      <c r="BC9" t="s">
-        <v>234</v>
-      </c>
       <c r="BD9" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE9" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI9">
         <v>2.5</v>
@@ -3875,28 +3875,28 @@
         <v>64</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="I10" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J10" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K10" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L10" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M10" s="30" t="s">
         <v>40</v>
@@ -3908,55 +3908,55 @@
         <v>21959015</v>
       </c>
       <c r="P10" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q10" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="Q10" s="57" t="s">
-        <v>138</v>
-      </c>
       <c r="R10" t="s">
         <v>40</v>
       </c>
       <c r="S10" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V10" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W10" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X10" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y10" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z10" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W10" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X10" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y10" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z10" s="58" t="s">
+      <c r="AA10" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA10" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC10" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD10" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE10" s="56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AF10" s="53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG10" s="53">
         <v>7.8838872528397141</v>
@@ -3966,13 +3966,13 @@
         <v>40</v>
       </c>
       <c r="AJ10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK10" t="s">
         <v>3</v>
       </c>
       <c r="AL10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM10" t="s">
         <v>58</v>
@@ -3981,10 +3981,10 @@
         <v>4</v>
       </c>
       <c r="AO10" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ10">
         <v>124</v>
@@ -3993,16 +3993,16 @@
         <v>124</v>
       </c>
       <c r="AT10" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU10" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU10" s="55" t="s">
+      <c r="AV10" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV10" s="55" t="s">
+      <c r="AW10" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW10" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY10" s="24">
         <v>40255</v>
@@ -4014,22 +4014,22 @@
         <v>12.270827000000001</v>
       </c>
       <c r="BB10" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC10" t="s">
         <v>233</v>
       </c>
-      <c r="BC10" t="s">
-        <v>234</v>
-      </c>
       <c r="BD10" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE10" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BI10">
         <v>3.5</v>
@@ -4068,28 +4068,28 @@
         <v>64</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="I11" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I11" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J11" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K11" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L11" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M11" s="30" t="s">
         <v>40</v>
@@ -4101,55 +4101,55 @@
         <v>19349699</v>
       </c>
       <c r="P11" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q11" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="Q11" s="57" t="s">
-        <v>140</v>
-      </c>
       <c r="R11" t="s">
         <v>40</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V11" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W11" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X11" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y11" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z11" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W11" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X11" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y11" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z11" s="58" t="s">
+      <c r="AA11" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA11" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC11" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD11" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE11" s="56" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF11" s="53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AG11" s="53">
         <v>11.490566648328533</v>
@@ -4159,13 +4159,13 @@
         <v>40</v>
       </c>
       <c r="AJ11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK11" t="s">
         <v>3</v>
       </c>
       <c r="AL11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM11" t="s">
         <v>58</v>
@@ -4174,10 +4174,10 @@
         <v>4</v>
       </c>
       <c r="AO11" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ11">
         <v>124</v>
@@ -4186,16 +4186,16 @@
         <v>124</v>
       </c>
       <c r="AT11" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU11" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU11" s="55" t="s">
+      <c r="AV11" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV11" s="55" t="s">
+      <c r="AW11" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW11" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY11" s="24">
         <v>40255</v>
@@ -4207,22 +4207,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC11" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD11" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE11" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF11" t="s">
         <v>236</v>
       </c>
-      <c r="BD11" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE11" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF11" t="s">
+      <c r="BG11" t="s">
         <v>238</v>
-      </c>
-      <c r="BG11" t="s">
-        <v>240</v>
       </c>
       <c r="BI11">
         <v>0.6</v>
@@ -4261,28 +4261,28 @@
         <v>64</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="I12" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J12" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K12" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L12" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M12" s="30" t="s">
         <v>40</v>
@@ -4294,55 +4294,55 @@
         <v>24640452</v>
       </c>
       <c r="P12" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q12" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="Q12" s="57" t="s">
-        <v>142</v>
-      </c>
       <c r="R12" t="s">
         <v>40</v>
       </c>
       <c r="S12" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T12" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V12" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W12" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X12" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y12" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z12" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W12" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X12" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y12" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z12" s="58" t="s">
+      <c r="AA12" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA12" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC12" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD12" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE12" s="56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF12" s="53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AG12" s="53">
         <v>4.5328630141419373</v>
@@ -4352,13 +4352,13 @@
         <v>40</v>
       </c>
       <c r="AJ12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK12" t="s">
         <v>3</v>
       </c>
       <c r="AL12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM12" t="s">
         <v>58</v>
@@ -4367,10 +4367,10 @@
         <v>4</v>
       </c>
       <c r="AO12" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ12">
         <v>124</v>
@@ -4379,16 +4379,16 @@
         <v>124</v>
       </c>
       <c r="AT12" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU12" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU12" s="55" t="s">
+      <c r="AV12" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV12" s="55" t="s">
+      <c r="AW12" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW12" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY12" s="24">
         <v>40255</v>
@@ -4400,22 +4400,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC12" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD12" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE12" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF12" t="s">
         <v>236</v>
       </c>
-      <c r="BD12" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF12" t="s">
+      <c r="BG12" t="s">
         <v>238</v>
-      </c>
-      <c r="BG12" t="s">
-        <v>240</v>
       </c>
       <c r="BI12">
         <v>0.8</v>
@@ -4454,28 +4454,28 @@
         <v>64</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="I13" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J13" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K13" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L13" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M13" s="30" t="s">
         <v>40</v>
@@ -4487,55 +4487,55 @@
         <v>22292795</v>
       </c>
       <c r="P13" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q13" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" s="57" t="s">
-        <v>144</v>
-      </c>
       <c r="R13" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T13" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V13" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W13" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X13" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y13" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z13" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W13" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X13" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y13" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z13" s="58" t="s">
+      <c r="AA13" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA13" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC13" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD13" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE13" s="56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF13" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AG13" s="53">
         <v>12.054733935255602</v>
@@ -4545,13 +4545,13 @@
         <v>40</v>
       </c>
       <c r="AJ13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK13" t="s">
         <v>3</v>
       </c>
       <c r="AL13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM13" t="s">
         <v>58</v>
@@ -4560,10 +4560,10 @@
         <v>4</v>
       </c>
       <c r="AO13" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ13">
         <v>124</v>
@@ -4572,16 +4572,16 @@
         <v>124</v>
       </c>
       <c r="AT13" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU13" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU13" s="55" t="s">
+      <c r="AV13" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV13" s="55" t="s">
+      <c r="AW13" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW13" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY13" s="24">
         <v>40255</v>
@@ -4593,22 +4593,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC13" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD13" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF13" t="s">
         <v>236</v>
       </c>
-      <c r="BD13" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE13" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF13" t="s">
+      <c r="BG13" t="s">
         <v>238</v>
-      </c>
-      <c r="BG13" t="s">
-        <v>240</v>
       </c>
       <c r="BI13">
         <v>1</v>
@@ -4647,28 +4647,28 @@
         <v>64</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="I14" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J14" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K14" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L14" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L14" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>40</v>
@@ -4680,55 +4680,55 @@
         <v>24336672</v>
       </c>
       <c r="P14" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q14" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="Q14" s="57" t="s">
-        <v>146</v>
-      </c>
       <c r="R14" t="s">
         <v>40</v>
       </c>
       <c r="S14" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T14" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V14" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W14" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X14" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y14" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z14" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W14" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X14" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y14" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z14" s="58" t="s">
+      <c r="AA14" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA14" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC14" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD14" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE14" s="56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF14" s="53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AG14" s="53">
         <v>1.6402921156812615</v>
@@ -4738,13 +4738,13 @@
         <v>40</v>
       </c>
       <c r="AJ14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK14" t="s">
         <v>3</v>
       </c>
       <c r="AL14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM14" t="s">
         <v>58</v>
@@ -4753,10 +4753,10 @@
         <v>4</v>
       </c>
       <c r="AO14" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ14">
         <v>124</v>
@@ -4765,16 +4765,16 @@
         <v>124</v>
       </c>
       <c r="AT14" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU14" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU14" s="55" t="s">
+      <c r="AV14" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV14" s="55" t="s">
+      <c r="AW14" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW14" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY14" s="24">
         <v>40255</v>
@@ -4786,22 +4786,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC14" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD14" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE14" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF14" t="s">
         <v>236</v>
       </c>
-      <c r="BD14" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE14" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF14" t="s">
+      <c r="BG14" t="s">
         <v>238</v>
-      </c>
-      <c r="BG14" t="s">
-        <v>240</v>
       </c>
       <c r="BI14">
         <v>1.2</v>
@@ -4840,28 +4840,28 @@
         <v>64</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="I15" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J15" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K15" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L15" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L15" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M15" s="30" t="s">
         <v>40</v>
@@ -4873,55 +4873,55 @@
         <v>22153770</v>
       </c>
       <c r="P15" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q15" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="Q15" s="57" t="s">
-        <v>148</v>
-      </c>
       <c r="R15" t="s">
         <v>40</v>
       </c>
       <c r="S15" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T15" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V15" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W15" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X15" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y15" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z15" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W15" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X15" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y15" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z15" s="58" t="s">
+      <c r="AA15" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA15" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC15" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD15" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE15" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF15" s="53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AG15" s="53">
         <v>4.9535613734183368</v>
@@ -4931,13 +4931,13 @@
         <v>40</v>
       </c>
       <c r="AJ15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK15" t="s">
         <v>3</v>
       </c>
       <c r="AL15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM15" t="s">
         <v>58</v>
@@ -4946,10 +4946,10 @@
         <v>4</v>
       </c>
       <c r="AO15" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ15">
         <v>124</v>
@@ -4958,16 +4958,16 @@
         <v>124</v>
       </c>
       <c r="AT15" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU15" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU15" s="55" t="s">
+      <c r="AV15" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV15" s="55" t="s">
+      <c r="AW15" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW15" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY15" s="24">
         <v>40255</v>
@@ -4979,22 +4979,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC15" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD15" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF15" t="s">
         <v>236</v>
       </c>
-      <c r="BD15" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE15" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF15" t="s">
+      <c r="BG15" t="s">
         <v>238</v>
-      </c>
-      <c r="BG15" t="s">
-        <v>240</v>
       </c>
       <c r="BI15">
         <v>1.5</v>
@@ -5033,28 +5033,28 @@
         <v>64</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G16" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="I16" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J16" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L16" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M16" s="30" t="s">
         <v>40</v>
@@ -5066,55 +5066,55 @@
         <v>23514431</v>
       </c>
       <c r="P16" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q16" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="Q16" s="57" t="s">
-        <v>150</v>
-      </c>
       <c r="R16" t="s">
         <v>40</v>
       </c>
       <c r="S16" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T16" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V16" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W16" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X16" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y16" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z16" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W16" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X16" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y16" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z16" s="58" t="s">
+      <c r="AA16" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA16" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC16" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD16" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE16" s="56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF16" s="53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AG16" s="53">
         <v>3.3484353257176145</v>
@@ -5124,13 +5124,13 @@
         <v>40</v>
       </c>
       <c r="AJ16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK16" t="s">
         <v>3</v>
       </c>
       <c r="AL16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM16" t="s">
         <v>58</v>
@@ -5139,10 +5139,10 @@
         <v>4</v>
       </c>
       <c r="AO16" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ16">
         <v>124</v>
@@ -5151,16 +5151,16 @@
         <v>124</v>
       </c>
       <c r="AT16" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU16" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU16" s="55" t="s">
+      <c r="AV16" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV16" s="55" t="s">
+      <c r="AW16" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW16" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY16" s="24">
         <v>40255</v>
@@ -5172,22 +5172,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC16" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD16" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE16" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF16" t="s">
         <v>236</v>
       </c>
-      <c r="BD16" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE16" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF16" t="s">
+      <c r="BG16" t="s">
         <v>238</v>
-      </c>
-      <c r="BG16" t="s">
-        <v>240</v>
       </c>
       <c r="BI16">
         <v>1.8</v>
@@ -5226,28 +5226,28 @@
         <v>64</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G17" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="I17" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J17" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K17" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L17" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M17" s="30" t="s">
         <v>40</v>
@@ -5259,55 +5259,55 @@
         <v>25239007</v>
       </c>
       <c r="P17" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q17" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="Q17" s="57" t="s">
-        <v>152</v>
-      </c>
       <c r="R17" t="s">
         <v>40</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T17" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V17" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W17" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X17" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y17" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z17" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W17" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X17" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y17" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z17" s="58" t="s">
+      <c r="AA17" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA17" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC17" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD17" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE17" s="56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF17" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG17" s="53">
         <v>2.2605525171785161</v>
@@ -5317,13 +5317,13 @@
         <v>40</v>
       </c>
       <c r="AJ17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK17" t="s">
         <v>3</v>
       </c>
       <c r="AL17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM17" t="s">
         <v>58</v>
@@ -5332,10 +5332,10 @@
         <v>4</v>
       </c>
       <c r="AO17" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ17">
         <v>124</v>
@@ -5344,16 +5344,16 @@
         <v>124</v>
       </c>
       <c r="AT17" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU17" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU17" s="55" t="s">
+      <c r="AV17" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV17" s="55" t="s">
+      <c r="AW17" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW17" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY17" s="24">
         <v>40255</v>
@@ -5365,22 +5365,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC17" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD17" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE17" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF17" t="s">
         <v>236</v>
       </c>
-      <c r="BD17" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE17" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF17" t="s">
+      <c r="BG17" t="s">
         <v>238</v>
-      </c>
-      <c r="BG17" t="s">
-        <v>240</v>
       </c>
       <c r="BI17">
         <v>2.2999999999999998</v>
@@ -5419,28 +5419,28 @@
         <v>64</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="I18" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J18" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K18" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L18" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L18" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M18" s="30" t="s">
         <v>40</v>
@@ -5452,55 +5452,55 @@
         <v>26888537</v>
       </c>
       <c r="P18" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q18" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="Q18" s="57" t="s">
-        <v>154</v>
-      </c>
       <c r="R18" t="s">
         <v>40</v>
       </c>
       <c r="S18" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T18" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V18" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W18" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X18" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y18" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z18" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W18" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X18" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y18" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z18" s="58" t="s">
+      <c r="AA18" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA18" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC18" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD18" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE18" s="56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF18" s="53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AG18" s="53">
         <v>7.3035392597866311</v>
@@ -5510,13 +5510,13 @@
         <v>40</v>
       </c>
       <c r="AJ18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK18" t="s">
         <v>3</v>
       </c>
       <c r="AL18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM18" t="s">
         <v>58</v>
@@ -5525,10 +5525,10 @@
         <v>4</v>
       </c>
       <c r="AO18" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ18">
         <v>124</v>
@@ -5537,16 +5537,16 @@
         <v>124</v>
       </c>
       <c r="AT18" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU18" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU18" s="55" t="s">
+      <c r="AV18" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV18" s="55" t="s">
+      <c r="AW18" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW18" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY18" s="24">
         <v>40256</v>
@@ -5558,22 +5558,22 @@
         <v>12.548028</v>
       </c>
       <c r="BB18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC18" t="s">
+        <v>234</v>
+      </c>
+      <c r="BD18" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE18" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF18" t="s">
         <v>236</v>
       </c>
-      <c r="BD18" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="BE18" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BF18" t="s">
+      <c r="BG18" t="s">
         <v>238</v>
-      </c>
-      <c r="BG18" t="s">
-        <v>240</v>
       </c>
       <c r="BI18">
         <v>2.6</v>
@@ -5612,28 +5612,28 @@
         <v>64</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="H19" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="I19" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J19" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K19" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L19" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L19" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M19" s="30" t="s">
         <v>40</v>
@@ -5645,55 +5645,55 @@
         <v>24099741</v>
       </c>
       <c r="P19" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q19" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="Q19" s="57" t="s">
-        <v>156</v>
-      </c>
       <c r="R19" t="s">
         <v>40</v>
       </c>
       <c r="S19" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T19" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V19" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W19" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X19" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y19" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z19" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W19" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X19" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y19" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z19" s="58" t="s">
+      <c r="AA19" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA19" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC19" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD19" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE19" s="56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AF19" s="53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AG19" s="53">
         <v>1.7233530737948071</v>
@@ -5703,13 +5703,13 @@
         <v>40</v>
       </c>
       <c r="AJ19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK19" t="s">
         <v>3</v>
       </c>
       <c r="AL19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM19" t="s">
         <v>58</v>
@@ -5718,10 +5718,10 @@
         <v>4</v>
       </c>
       <c r="AO19" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ19">
         <v>124</v>
@@ -5730,16 +5730,16 @@
         <v>124</v>
       </c>
       <c r="AT19" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU19" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU19" s="55" t="s">
+      <c r="AV19" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV19" s="55" t="s">
+      <c r="AW19" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW19" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY19" s="24">
         <v>40256</v>
@@ -5751,22 +5751,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD19" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE19" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI19">
         <v>0.45</v>
@@ -5803,28 +5803,28 @@
         <v>64</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="H20" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="I20" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J20" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K20" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L20" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L20" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M20" s="30" t="s">
         <v>40</v>
@@ -5836,55 +5836,55 @@
         <v>25131709</v>
       </c>
       <c r="P20" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q20" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="Q20" s="57" t="s">
-        <v>158</v>
-      </c>
       <c r="R20" t="s">
         <v>40</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T20" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V20" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W20" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X20" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y20" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z20" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W20" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X20" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y20" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z20" s="58" t="s">
+      <c r="AA20" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA20" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC20" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD20" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE20" s="56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AF20" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG20" s="53">
         <v>2.1834244846445099</v>
@@ -5894,13 +5894,13 @@
         <v>40</v>
       </c>
       <c r="AJ20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK20" t="s">
         <v>3</v>
       </c>
       <c r="AL20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM20" t="s">
         <v>58</v>
@@ -5909,10 +5909,10 @@
         <v>4</v>
       </c>
       <c r="AO20" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ20">
         <v>124</v>
@@ -5921,16 +5921,16 @@
         <v>124</v>
       </c>
       <c r="AT20" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU20" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU20" s="55" t="s">
+      <c r="AV20" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV20" s="55" t="s">
+      <c r="AW20" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW20" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY20" s="24">
         <v>40256</v>
@@ -5942,22 +5942,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD20" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE20" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI20">
         <v>0.75</v>
@@ -5994,28 +5994,28 @@
         <v>64</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="H21" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="I21" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I21" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J21" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L21" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L21" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M21" s="30" t="s">
         <v>40</v>
@@ -6027,55 +6027,55 @@
         <v>25333059</v>
       </c>
       <c r="P21" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q21" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="Q21" s="57" t="s">
-        <v>160</v>
-      </c>
       <c r="R21" t="s">
         <v>40</v>
       </c>
       <c r="S21" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T21" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V21" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W21" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X21" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y21" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z21" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W21" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X21" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y21" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z21" s="58" t="s">
+      <c r="AA21" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA21" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC21" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD21" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE21" s="56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AF21" s="53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG21" s="53">
         <v>2.8624747850662868</v>
@@ -6085,13 +6085,13 @@
         <v>40</v>
       </c>
       <c r="AJ21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK21" t="s">
         <v>3</v>
       </c>
       <c r="AL21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM21" t="s">
         <v>58</v>
@@ -6100,10 +6100,10 @@
         <v>4</v>
       </c>
       <c r="AO21" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ21">
         <v>124</v>
@@ -6112,16 +6112,16 @@
         <v>124</v>
       </c>
       <c r="AT21" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU21" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU21" s="55" t="s">
+      <c r="AV21" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV21" s="55" t="s">
+      <c r="AW21" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW21" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY21" s="24">
         <v>40256</v>
@@ -6133,22 +6133,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD21" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE21" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI21">
         <v>1.05</v>
@@ -6185,28 +6185,28 @@
         <v>64</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="H22" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="I22" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I22" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J22" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K22" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L22" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M22" s="30" t="s">
         <v>40</v>
@@ -6218,55 +6218,55 @@
         <v>23643065</v>
       </c>
       <c r="P22" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q22" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="Q22" s="57" t="s">
-        <v>162</v>
-      </c>
       <c r="R22" t="s">
         <v>40</v>
       </c>
       <c r="S22" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V22" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W22" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X22" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y22" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z22" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W22" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X22" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y22" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z22" s="58" t="s">
+      <c r="AA22" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA22" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC22" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD22" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE22" s="56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AF22" s="53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG22" s="53">
         <v>6.1493155561308699</v>
@@ -6276,13 +6276,13 @@
         <v>40</v>
       </c>
       <c r="AJ22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK22" t="s">
         <v>3</v>
       </c>
       <c r="AL22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM22" t="s">
         <v>58</v>
@@ -6291,10 +6291,10 @@
         <v>4</v>
       </c>
       <c r="AO22" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ22">
         <v>124</v>
@@ -6303,16 +6303,16 @@
         <v>124</v>
       </c>
       <c r="AT22" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU22" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU22" s="55" t="s">
+      <c r="AV22" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV22" s="55" t="s">
+      <c r="AW22" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW22" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY22" s="24">
         <v>40256</v>
@@ -6324,22 +6324,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD22" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE22" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI22">
         <v>1.35</v>
@@ -6376,28 +6376,28 @@
         <v>64</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="H23" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="I23" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I23" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J23" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K23" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L23" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L23" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M23" s="30" t="s">
         <v>40</v>
@@ -6409,55 +6409,55 @@
         <v>23126069</v>
       </c>
       <c r="P23" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q23" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="Q23" s="57" t="s">
-        <v>164</v>
-      </c>
       <c r="R23" t="s">
         <v>40</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T23" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V23" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W23" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X23" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y23" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z23" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W23" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X23" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y23" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z23" s="58" t="s">
+      <c r="AA23" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA23" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC23" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD23" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE23" s="56" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF23" s="53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AG23" s="53">
         <v>11.453890381109566</v>
@@ -6467,13 +6467,13 @@
         <v>40</v>
       </c>
       <c r="AJ23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK23" t="s">
         <v>3</v>
       </c>
       <c r="AL23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM23" t="s">
         <v>58</v>
@@ -6482,10 +6482,10 @@
         <v>4</v>
       </c>
       <c r="AO23" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ23">
         <v>124</v>
@@ -6494,16 +6494,16 @@
         <v>124</v>
       </c>
       <c r="AT23" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU23" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU23" s="55" t="s">
+      <c r="AV23" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV23" s="55" t="s">
+      <c r="AW23" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW23" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY23" s="24">
         <v>40256</v>
@@ -6515,22 +6515,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD23" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE23" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI23">
         <v>1.95</v>
@@ -6567,28 +6567,28 @@
         <v>64</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="H24" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="I24" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J24" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K24" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="L24" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L24" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M24" s="30" t="s">
         <v>40</v>
@@ -6600,55 +6600,55 @@
         <v>21665592</v>
       </c>
       <c r="P24" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q24" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="Q24" s="57" t="s">
-        <v>166</v>
-      </c>
       <c r="R24" t="s">
         <v>40</v>
       </c>
       <c r="S24" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T24" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="V24" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W24" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="X24" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y24" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z24" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W24" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X24" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y24" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z24" s="58" t="s">
+      <c r="AA24" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA24" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC24" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD24" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE24" s="56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF24" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AG24" s="53">
         <v>4.059847038391422</v>
@@ -6658,13 +6658,13 @@
         <v>40</v>
       </c>
       <c r="AJ24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK24" t="s">
         <v>3</v>
       </c>
       <c r="AL24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM24" t="s">
         <v>58</v>
@@ -6673,10 +6673,10 @@
         <v>4</v>
       </c>
       <c r="AO24" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ24">
         <v>124</v>
@@ -6685,16 +6685,16 @@
         <v>124</v>
       </c>
       <c r="AT24" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU24" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU24" s="55" t="s">
+      <c r="AV24" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV24" s="55" t="s">
+      <c r="AW24" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW24" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY24" s="24">
         <v>40256</v>
@@ -6706,22 +6706,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD24" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE24" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI24">
         <v>2.95</v>
@@ -6758,28 +6758,28 @@
         <v>64</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="H25" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="I25" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I25" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="J25" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K25" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="K25" s="57" t="s">
+      <c r="L25" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="L25" s="57" t="s">
-        <v>122</v>
       </c>
       <c r="M25" s="30" t="s">
         <v>40</v>
@@ -6791,55 +6791,55 @@
         <v>24804911</v>
       </c>
       <c r="P25" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q25" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="Q25" s="57" t="s">
+      <c r="R25" t="s">
+        <v>40</v>
+      </c>
+      <c r="S25" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="T25" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="R25" t="s">
-        <v>40</v>
-      </c>
-      <c r="S25" s="16" t="s">
+      <c r="U25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V25" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="W25" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="T25" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V25" s="33" t="s">
+      <c r="X25" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y25" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z25" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="W25" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="X25" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y25" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z25" s="58" t="s">
+      <c r="AA25" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="AA25" s="54" t="s">
-        <v>196</v>
-      </c>
       <c r="AB25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AC25" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AD25" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE25" s="56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF25" s="53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AG25" s="53">
         <v>3.7195128528742329</v>
@@ -6849,13 +6849,13 @@
         <v>40</v>
       </c>
       <c r="AJ25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK25" t="s">
         <v>3</v>
       </c>
       <c r="AL25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM25" t="s">
         <v>58</v>
@@ -6864,10 +6864,10 @@
         <v>4</v>
       </c>
       <c r="AO25" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="AP25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ25">
         <v>124</v>
@@ -6876,16 +6876,16 @@
         <v>124</v>
       </c>
       <c r="AT25" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU25" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="AU25" s="55" t="s">
+      <c r="AV25" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="AV25" s="55" t="s">
+      <c r="AW25" s="55" t="s">
         <v>231</v>
-      </c>
-      <c r="AW25" s="55" t="s">
-        <v>232</v>
       </c>
       <c r="AY25" s="24">
         <v>40256</v>
@@ -6897,22 +6897,22 @@
         <v>14.458780000000001</v>
       </c>
       <c r="BB25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BD25" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="BE25" s="25" t="s">
         <v>40</v>
       </c>
       <c r="BF25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BG25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BI25">
         <v>3.25</v>
@@ -6939,19 +6939,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -6969,14 +6959,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>